<commit_message>
april weekly status report added
</commit_message>
<xml_diff>
--- a/april_status/Pavan_sonwane _april.xlsx
+++ b/april_status/Pavan_sonwane _april.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="10 april to 17 april" sheetId="2" r:id="rId1"/>
-    <sheet name="18 april to 24 april" sheetId="3" r:id="rId2"/>
+    <sheet name="3 april to 9 april" sheetId="4" r:id="rId1"/>
+    <sheet name="10 april to 17 april" sheetId="2" r:id="rId2"/>
+    <sheet name="18 april to 24 april" sheetId="3" r:id="rId3"/>
+    <sheet name="25 april to 30 april" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="91">
   <si>
     <t>DATE</t>
   </si>
@@ -208,13 +209,94 @@
   </si>
   <si>
     <t xml:space="preserve">practice excel  &amp; email </t>
+  </si>
+  <si>
+    <t>Git command uses /how to work</t>
+  </si>
+  <si>
+    <t>Git command -help,rm,restore --stageed</t>
+  </si>
+  <si>
+    <t>01:00 Hrs</t>
+  </si>
+  <si>
+    <t>30:00 min</t>
+  </si>
+  <si>
+    <t>Parctice</t>
+  </si>
+  <si>
+    <t>Email parctice</t>
+  </si>
+  <si>
+    <t>Linux command parctice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel sheet edit </t>
+  </si>
+  <si>
+    <t>parctice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Hrs </t>
+  </si>
+  <si>
+    <t>8 Hrs</t>
+  </si>
+  <si>
+    <t>19 Hrs</t>
+  </si>
+  <si>
+    <t>Application support enngginer basice informaition</t>
+  </si>
+  <si>
+    <t>Virtaul Box &amp; Ubuntu  guid installation</t>
+  </si>
+  <si>
+    <t>Pending installation</t>
+  </si>
+  <si>
+    <t>Ubuntu installation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off </t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>4 Hrs</t>
+  </si>
+  <si>
+    <t>0 Hrs</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>25:30 Hrs</t>
+  </si>
+  <si>
+    <t>Virtaul Box &amp; Ubuntu /linux installation</t>
+  </si>
+  <si>
+    <t>Linux notes refer</t>
+  </si>
+  <si>
+    <t>Git command / create repositary and branch create and clone branch</t>
+  </si>
+  <si>
+    <t>VCS repositary/branch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,16 +324,75 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -379,11 +520,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -431,6 +626,107 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -697,7 +993,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,10 +1001,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3:I18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6">
+        <v>44654</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44660</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7">
+        <v>44652</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" ht="15.75">
+      <c r="B10" s="12"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="2:9" ht="30">
+      <c r="B11" s="1"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="13">
+        <v>44654</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="1"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="13">
+        <v>44655</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="1"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="13">
+        <v>44656</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="1"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="13">
+        <v>44657</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="1"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="13">
+        <v>44658</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="1"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="13">
+        <v>44659</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="1"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="13">
+        <v>44660</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B18" s="1"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,7 +1338,9 @@
       <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:7">
@@ -799,10 +1404,10 @@
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="9"/>
@@ -812,16 +1417,16 @@
     </row>
     <row r="8" spans="2:7" s="12" customFormat="1" ht="15.75">
       <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="62" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="25" t="s">
@@ -878,7 +1483,7 @@
       <c r="F11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -968,7 +1573,7 @@
       <c r="F16" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="72" t="s">
         <v>25</v>
       </c>
     </row>
@@ -978,12 +1583,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1015,7 +1623,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="27" t="s">
@@ -1229,4 +1837,319 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B5:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B5" s="9"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="73"/>
+      <c r="C6" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="46"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="73"/>
+      <c r="C7" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="48">
+        <v>4</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="73"/>
+      <c r="C8" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="52">
+        <v>44676</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="51"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="73"/>
+      <c r="C9" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="52">
+        <v>44681</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="51"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="73"/>
+      <c r="C10" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="53">
+        <v>44652</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="73"/>
+      <c r="C11" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75">
+      <c r="B12" s="74"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="2:9" ht="30">
+      <c r="B13" s="73"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32">
+        <v>44676</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="73"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32">
+        <v>44677</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="73"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32">
+        <v>44678</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" ht="30">
+      <c r="B16" s="73"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32">
+        <v>44679</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="73"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32">
+        <v>44680</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="73"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32">
+        <v>44681</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="73"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B20" s="73"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="70"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>